<commit_message>
Update ToDo y StackWeapon
</commit_message>
<xml_diff>
--- a/Bibliografía/ToDO.xlsx
+++ b/Bibliografía/ToDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDLABU2\Bibliografía\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A81656-2C73-4706-BDAD-793D1728C3E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB6FEE-54BA-4E9D-8C82-ED267F0A87CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{16073332-0623-4256-8703-3FEB2668B41D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>Matchmaking</t>
   </si>
@@ -128,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,11 +163,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -160,36 +179,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -535,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBBB93B-9557-45BC-94BB-181B3A3F250C}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,13 +537,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
@@ -562,16 +552,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
@@ -579,16 +569,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -596,16 +586,16 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G4" t="s">
@@ -613,100 +603,122 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D19 G3">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Listo paso 4 para matchmaking
</commit_message>
<xml_diff>
--- a/Bibliografía/ToDO.xlsx
+++ b/Bibliografía/ToDO.xlsx
@@ -5,25 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDLABU2\Bibliografía\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\AEDLABU2\Bibliografía\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB6FEE-54BA-4E9D-8C82-ED267F0A87CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FDC9B6-1894-4FF2-865B-A85B66A4A10B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{16073332-0623-4256-8703-3FEB2668B41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -525,7 +520,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +602,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Listo metodo de ing para matchmaking
</commit_message>
<xml_diff>
--- a/Bibliografía/ToDO.xlsx
+++ b/Bibliografía/ToDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\AEDLABU2\Bibliografía\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FDC9B6-1894-4FF2-865B-A85B66A4A10B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18311DE2-7BB1-4A32-AEA6-96EC347A3812}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{16073332-0623-4256-8703-3FEB2668B41D}"/>
   </bookViews>
@@ -166,7 +166,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -520,14 +550,14 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="1"/>
+    <col min="3" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -619,7 +649,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
@@ -664,7 +694,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
@@ -706,19 +736,30 @@
       <c r="J11" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D19 G3">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="B2:D18 G3 B19:C19">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:J11">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Empezado diseño de pruebas TestMatchmaking
</commit_message>
<xml_diff>
--- a/Bibliografía/ToDO.xlsx
+++ b/Bibliografía/ToDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDLABU2\Bibliografía\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4E076F-2E31-4489-BE2D-9EFC19100051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB742AA9-B54F-4F46-AA82-766A9C4BAB60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{16073332-0623-4256-8703-3FEB2668B41D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Matchmaking</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Diseños preliminares</t>
-  </si>
-  <si>
-    <t>n</t>
   </si>
   <si>
     <t>Selección de la mejor solucion</t>
@@ -166,7 +163,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -550,7 +627,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +652,7 @@
       <c r="G1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -592,6 +670,7 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -609,6 +688,9 @@
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -618,7 +700,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>5</v>
@@ -626,6 +708,7 @@
       <c r="G4" t="s">
         <v>9</v>
       </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -635,41 +718,45 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -677,13 +764,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
@@ -691,7 +778,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>5</v>
@@ -705,31 +792,31 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -737,29 +824,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D18 G3 B19:C19">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:J11">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H6">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Juntando todo en el informe
</commit_message>
<xml_diff>
--- a/Bibliografía/ToDO.xlsx
+++ b/Bibliografía/ToDO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDLABU2\Bibliografía\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB742AA9-B54F-4F46-AA82-766A9C4BAB60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B978865A-AC13-4606-9E82-5A010B99D434}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{16073332-0623-4256-8703-3FEB2668B41D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Matchmaking</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">Búsqueda de soluciones </t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
   <si>
     <t>Diseños preliminares</t>
@@ -163,7 +160,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -171,76 +168,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -626,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBBB93B-9557-45BC-94BB-181B3A3F250C}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="JA1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +597,9 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -712,19 +641,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>5</v>
@@ -732,25 +661,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
@@ -764,10 +693,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>5</v>
@@ -778,7 +707,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>5</v>
@@ -792,10 +721,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>5</v>
@@ -805,18 +734,18 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -824,29 +753,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D18 G3 B19:C19">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:J11">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>